<commit_message>
add convert format from excel
</commit_message>
<xml_diff>
--- a/samples/RxBim.Tools.TableBuilder.Excel.Sample/excel/sample1.xlsx
+++ b/samples/RxBim.Tools.TableBuilder.Excel.Sample/excel/sample1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavlo\OneDrive\Документы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavlo\RiderProjects\RxBim.Tools\samples\RxBim.Tools.TableBuilder.Excel.Sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C546362-6B0B-4418-9ABE-1491FBF71272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC4263-C327-4EF3-87F7-2936DC295DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{863EC02E-3F17-485F-854B-E2425759C84C}"/>
   </bookViews>
@@ -57,23 +57,34 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -81,13 +92,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,126 +468,126 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <f>SUM(A2,B2)</f>
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C10" si="0">SUM(A3,B3)</f>
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>

</xml_diff>